<commit_message>
Add model for JournalEntry and add func to front end
</commit_message>
<xml_diff>
--- a/passport/passport_trips.xlsx
+++ b/passport/passport_trips.xlsx
@@ -16,14 +16,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +48,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +429,214 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>visited</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>start_date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>end_date</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Athens</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45981</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>45988</v>
+      </c>
+      <c r="F2" t="n">
+        <v>37.9755648</v>
+      </c>
+      <c r="G2" t="n">
+        <v>23.7348324</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Athens</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45981</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45988</v>
+      </c>
+      <c r="F3" t="n">
+        <v>37.9755648</v>
+      </c>
+      <c r="G3" t="n">
+        <v>23.7348324</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Athens</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45981</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45988</v>
+      </c>
+      <c r="F4" t="n">
+        <v>37.9755648</v>
+      </c>
+      <c r="G4" t="n">
+        <v>23.7348324</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bogota</t>
+        </is>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45422</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45432</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.6533817</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-74.0836331</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bogota</t>
+        </is>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45422</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>45432</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.6533817</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-74.0836331</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Buenos Aires</t>
+        </is>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>46082</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>46090</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-34.6095579</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-58.3887904</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>